<commit_message>
CHARMS AUTOMATION - RAS SCREENER SUBMISSION USING EXCEL
</commit_message>
<xml_diff>
--- a/src/test/java/ServiceNow/CHARMS/Resources/SelfRasScreenerSubmissionScenario1.xlsx
+++ b/src/test/java/ServiceNow/CHARMS/Resources/SelfRasScreenerSubmissionScenario1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juarezds/Desktop/CBIIT-Test-Automation/src/test/java/ServiceNow/CHARMS/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E90274F-11B7-3B43-82E9-8E32766D899C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ACB84FC-B3A0-A341-8F8F-D2A7266EAB3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17480" xr2:uid="{54739BCC-024D-1B43-9BD3-233381306DEA}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17440" xr2:uid="{54739BCC-024D-1B43-9BD3-233381306DEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="62">
   <si>
     <t>Question</t>
   </si>
@@ -69,6 +69,159 @@
   </si>
   <si>
     <t>What is your date of birth?</t>
+  </si>
+  <si>
+    <t>Date of birth month</t>
+  </si>
+  <si>
+    <t>April</t>
+  </si>
+  <si>
+    <t>Date of birth year</t>
+  </si>
+  <si>
+    <t>What was your sex assigned at birth?</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Are you adopted?</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>In which country do you currently live?</t>
+  </si>
+  <si>
+    <t>United States of America</t>
+  </si>
+  <si>
+    <t>Please provide the mailing address where study materials can be sent, as needed.</t>
+  </si>
+  <si>
+    <t>Street</t>
+  </si>
+  <si>
+    <t>12-34 home address</t>
+  </si>
+  <si>
+    <t>Apt 600</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State (Abbreviation)</t>
+  </si>
+  <si>
+    <t>VA</t>
+  </si>
+  <si>
+    <t>Zip Code</t>
+  </si>
+  <si>
+    <t>Street 2 (optional)</t>
+  </si>
+  <si>
+    <t>What is your email address?</t>
+  </si>
+  <si>
+    <t>automatedTest@email.com</t>
+  </si>
+  <si>
+    <t>Please confirm your email address</t>
+  </si>
+  <si>
+    <t>Home phone number</t>
+  </si>
+  <si>
+    <t>Cell phone number</t>
+  </si>
+  <si>
+    <t>Work phone number</t>
+  </si>
+  <si>
+    <t>703-687-5816</t>
+  </si>
+  <si>
+    <t>What is your ethnicity?</t>
+  </si>
+  <si>
+    <t>Not Hispanic/Latino</t>
+  </si>
+  <si>
+    <t>Prefer not to answer</t>
+  </si>
+  <si>
+    <t>Are you a participant in any other research study or registry group?  Please specify.</t>
+  </si>
+  <si>
+    <t>I am not involved in any other research study or registry group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To determine eligibility for this study, we need to collect information about medical diagnoses.  These questions ask about general medical conditions, cancer and any prior diagnosis of a RASopathy.  Please complete this information to the best of your knowledge. </t>
+  </si>
+  <si>
+    <t>Have you ever been diagnosed with the following conditions?  Select all that apply.  If you do not see the exact condition diagnosed, please select the closest answer.</t>
+  </si>
+  <si>
+    <t>Never diagnosed with any of these conditions</t>
+  </si>
+  <si>
+    <t>Have you ever been diagnosed with cancer?</t>
+  </si>
+  <si>
+    <t>Have you been diagnosed with a RASopathy such as Noonan syndrome, Noonan syndrome with multiple lentigines, Costello syndrome, cardiofaciocutaneous syndrome, Legius syndrome, capillary arteriovenous malformation syndrome, hereditary gingival fibromatosis or SYNGAP1 syndrome?</t>
+  </si>
+  <si>
+    <t>We know that RASopathies are a group of syndromes that have a genetic basis.  In order to help us determine eligibility for the RASopathies Study, we also need to know about any genetic testing that has been completed.  We will need a copy of any test results.</t>
+  </si>
+  <si>
+    <t>Have any of your biological relatives been diagnosed with a RASopathy?</t>
+  </si>
+  <si>
+    <t>Have you ever had genetic testing?</t>
+  </si>
+  <si>
+    <t>We will now ask a few remaining questions regarding this study.</t>
+  </si>
+  <si>
+    <t>How did you hear about this study?  If a specific health care provider referred you to this study, please include their name in the corresponding text box.</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>How did you hear about this study?  If a specific health care provider referred you to this study, please include their name in the corresponding text box. Other reason</t>
+  </si>
+  <si>
+    <t>JUST TESTING</t>
+  </si>
+  <si>
+    <t>Have you or other family members ever participated in another study on RASopathies at another medical institution, university, government agency or other site?</t>
+  </si>
+  <si>
+    <t>What are the main reasons for participating in this study?  Select all that apply.  Please elaborate on the reason in the corresponding textbox.</t>
+  </si>
+  <si>
+    <t>TESTING REASONS</t>
+  </si>
+  <si>
+    <t>Burke</t>
+  </si>
+  <si>
+    <t>703-687-5814</t>
+  </si>
+  <si>
+    <t>703-687-5815</t>
+  </si>
+  <si>
+    <t>What is your race? Please select all that apply.</t>
+  </si>
+  <si>
+    <t>What are the main reasons for participating in this study?  Select all that apply.  Please elaborate on the reason in the corresponding textbox. Other reason</t>
   </si>
 </sst>
 </file>
@@ -76,9 +229,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="mm/dd/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="mm/dd/yyyy;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -90,6 +243,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -112,18 +273,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -436,23 +610,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AAA49E6-03DB-BC47-B34D-065780B05137}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -460,7 +634,7 @@
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -468,7 +642,7 @@
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -476,7 +650,7 @@
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -484,7 +658,7 @@
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -492,11 +666,259 @@
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="5">
         <v>32964</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1990</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="4">
+        <v>22015</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="136" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="85" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="153" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="136" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="85" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="85" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="85" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="85" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B18" r:id="rId1" xr:uid="{F82FA76E-2358-814A-8E85-BCB9636B476E}"/>
+    <hyperlink ref="B19" r:id="rId2" xr:uid="{9CF4B7EF-6998-144B-B594-2EFE15A9CFC2}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
CHARMS IIQ form partial updated automation
</commit_message>
<xml_diff>
--- a/src/test/java/ServiceNow/CHARMS/Resources/SelfRasScreenerSubmissionScenario1.xlsx
+++ b/src/test/java/ServiceNow/CHARMS/Resources/SelfRasScreenerSubmissionScenario1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bucurgb/IdeaProjects/CBIIT-Test-Automation/src/test/java/ServiceNow/CHARMS/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C43B93F0-0650-E248-88A6-D5352D679319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E0DE4CC-10CF-3B4C-B53C-8FF8030EB7F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="123320" yWindow="1780" windowWidth="30240" windowHeight="17440" activeTab="1" xr2:uid="{54739BCC-024D-1B43-9BD3-233381306DEA}"/>
+    <workbookView xWindow="45060" yWindow="-27940" windowWidth="26360" windowHeight="28120" activeTab="1" xr2:uid="{54739BCC-024D-1B43-9BD3-233381306DEA}"/>
   </bookViews>
   <sheets>
     <sheet name="screenerScenario1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="137">
   <si>
     <t>Question</t>
   </si>
@@ -250,10 +250,6 @@
     <t>Hispanic or Latino</t>
   </si>
   <si>
-    <t>What is your race? Please select all that
-apply.</t>
-  </si>
-  <si>
     <t>Black or African American</t>
   </si>
   <si>
@@ -261,10 +257,6 @@
   </si>
   <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>Were you raised primarily by someone 
-other than your biological (blood) parent?</t>
   </si>
   <si>
     <t>What is your date of birth?
@@ -282,41 +274,15 @@
 Year</t>
   </si>
   <si>
-    <t>Where were you born? If you do not 
-know, place an 'X' in the box next to 
-"don't know"
-City</t>
-  </si>
-  <si>
     <t>Bethesda</t>
   </si>
   <si>
-    <t>Where were you born? If you do not 
-know, place an 'X' in the box next to 
-"don't know"
-State/Province</t>
-  </si>
-  <si>
     <t>Maryland</t>
   </si>
   <si>
-    <t>Where were you born? If you do not 
-know, place an 'X' in the box next to 
-"don't know"
-Country</t>
-  </si>
-  <si>
     <t>United States</t>
   </si>
   <si>
-    <t>Where were you born? If you do not know, place an 'X' in the box next to "don't know"
-Don't know</t>
-  </si>
-  <si>
-    <t>Most people have ancestors who come from other parts of the world.  
-What is your biological mother's ancestral background? Please check all that apply.</t>
-  </si>
-  <si>
     <t>African</t>
   </si>
   <si>
@@ -344,10 +310,6 @@
     <t>Do you currently have health insurance?</t>
   </si>
   <si>
-    <t>What is the total combined yearly income for all the persons in your household?
-Include income from all sources such as wages, salaries, Social Security or retirement benefits, investments, help from relatives and so forth. Would you say your total combined income for your household in the last 12 months is...</t>
-  </si>
-  <si>
     <t>$60,001 - $80,000, or</t>
   </si>
   <si>
@@ -375,117 +337,13 @@
     <t>full term (37-42 weeks)</t>
   </si>
   <si>
-    <t>Please fill out your birth weight in the table below.
-Weight
-Numerical value
-(Estimate is OK)</t>
-  </si>
-  <si>
-    <t>Please fill out your birth weight in the table below.
-Unit of measure</t>
-  </si>
-  <si>
     <t>pounds</t>
   </si>
   <si>
-    <t>Please fill out your length and head 
-circumference at birth in the table below.
-Length
-Numerical value
-(Estimate is OK)</t>
-  </si>
-  <si>
-    <t>Please fill out your length and head 
-circumference at birth in the table below.
-Head circumference
-Numerical value
-(Estimate is OK)</t>
-  </si>
-  <si>
-    <t>Please fill out your length and head 
-circumference at birth in the table below.
-Length
-Unit of measure</t>
-  </si>
-  <si>
     <t>inches</t>
   </si>
   <si>
-    <t>Please fill out your length and head 
-circumference at birth in the table below.
-Head circumference
-Unit of measure</t>
-  </si>
-  <si>
     <t>centimeters</t>
-  </si>
-  <si>
-    <t>This section will ask about cancer and benign tumor history.
-Please fill out this information to the best of your knowledge.</t>
-  </si>
-  <si>
-    <t>Have you ever been diagnosed with any
-cancer and/or benign tumor?</t>
-  </si>
-  <si>
-    <t>Have you ever had medical genetic testing
-(excluding ancestry testing)?</t>
-  </si>
-  <si>
-    <t>Please complete the table below indicating your current height.
-Current height
-Numerical value
-(Estimate is OK)</t>
-  </si>
-  <si>
-    <t>Please complete the table below indicating your current height.
-Current height
-Please select unit of measure</t>
-  </si>
-  <si>
-    <t>Please complete the table below indicating your weight at the specified timepoints.
-Please do not include weights during
-pregnancy, if applicable.
-Current weight
-Numerical value
-(Estimate is OK)</t>
-  </si>
-  <si>
-    <t>Please complete the table below indicating your weight at the specified timepoints.
-Please do not include weights during
-pregnancy, if applicable.
-Highest weight during lifetime
-Numerical value
-(Estimate is OK)</t>
-  </si>
-  <si>
-    <t>Please complete the table below indicating your weight at the specified timepoints.
-Please do not include weights during
-pregnancy, if applicable.
-Weight at 18 years
-Numerical value
-(Estimate is OK)</t>
-  </si>
-  <si>
-    <t>Please complete the table below indicating your weight at the specified timepoints.
-Please do not include weights during
-pregnancy, if applicable.
-Current weight
-Please select unit of measure</t>
-  </si>
-  <si>
-    <t>Please complete the table below indicating your weight at the specified timepoints.
-Please do not include weights during
-pregnancy, if applicable.
-Highest weight during lifetime
-Please select unit of measure</t>
-  </si>
-  <si>
-    <t>Please complete the table below indicating your weight at the specified timepoints.
-Please do not include weights during
-pregnancy, if applicable.
-Weight at 18 years of age
-Please select unit of measure</t>
   </si>
   <si>
     <t>Please complete the table below indicating your weight at the specified timepoints.
@@ -504,15 +362,7 @@
 (for weight at 18, 30, and 40 years of age)</t>
   </si>
   <si>
-    <t>At what age were you at your highest
-weight?  Please specify if in months or years.</t>
-  </si>
-  <si>
     <t>16 years</t>
-  </si>
-  <si>
-    <t>Have you or your partner ever sought
-medical advice regarding fertility?</t>
   </si>
   <si>
     <t>You are almost done! 
@@ -542,6 +392,87 @@
   </si>
   <si>
     <t>What was your biological sex assigned at birth?</t>
+  </si>
+  <si>
+    <t>Were you raised primarily by someone other than your biological (blood) parent?</t>
+  </si>
+  <si>
+    <t>Where were you born? If you do not know, place an X in the box next to don't know City</t>
+  </si>
+  <si>
+    <t>Where were you born? If you do not know, place an X in the box next to don't know State</t>
+  </si>
+  <si>
+    <t>Where were you born? If you do not know, place an X in the box next to don't know Country</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Where were you born? If you do not know, place an X in the box next to don't know Country Don't know</t>
+  </si>
+  <si>
+    <t>Most people have ancestors who come from other parts of the world. What is your biological mother's ancestral background? Please check all that apply.</t>
+  </si>
+  <si>
+    <t>What is the total combined yearly income for all the persons in your household? Include income from all sources such as wages, salaries, Social Security or retirement benefits, investments, help from relatives and so forth. Would you say your total combined income for your household in the last 12 months is...</t>
+  </si>
+  <si>
+    <t>Please fill out your birth weight in the table below. WeightNumerical value (Estimate is OK)</t>
+  </si>
+  <si>
+    <t>Please fill out your birth weight in the table below. Unit of measure</t>
+  </si>
+  <si>
+    <t>Please fill out your length and head circumference at birth in the table below. Length Numerical value (Estimate is OK)</t>
+  </si>
+  <si>
+    <t>Please fill out your length and head circumference at birth in the table below. Unit of measure (Estimate is OK)</t>
+  </si>
+  <si>
+    <t>Please fill out your length and head circumference at birth in the table below. Head circumference numerical value (Estimate is OK)</t>
+  </si>
+  <si>
+    <t>Please fill out your length and head circumference at birth in the table below. Head circumference unit of measure (Estimate is OK)</t>
+  </si>
+  <si>
+    <t>This section will ask about cancer and benign tumor history. Please fill out this information to the best of your knowledge.</t>
+  </si>
+  <si>
+    <t>Have you ever been diagnosed with any cancer and/or benign tumor?</t>
+  </si>
+  <si>
+    <t>Have you ever had medical genetic testing (excluding ancestry testing)?</t>
+  </si>
+  <si>
+    <t>Please complete the table below indicating your current height. Current height Numerical value (Estimate is OK)</t>
+  </si>
+  <si>
+    <t>Please complete the table below indicating your current height. Current height unit of measure (Estimate is OK)</t>
+  </si>
+  <si>
+    <t>Please complete the table below indicating your weight at the specified time points. Please do not include weights during pregnancy, if applicable. Current weight Numerical value (Estimate is OK)</t>
+  </si>
+  <si>
+    <t>Please complete the table below indicating your weight at the specified time points. Please do not include weights during pregnancy, if applicable. Current weight unit of measure(Estimate is OK)</t>
+  </si>
+  <si>
+    <t>Please complete the table below indicating your weight at the specified time points. Please do not include weights during pregnancy, if applicable. During lifetime weight Numerical value (Estimate is OK)</t>
+  </si>
+  <si>
+    <t>Please complete the table below indicating your weight at the specified time points. Please do not include weights during pregnancy, if applicable.During lifetime weight unit of measure(Estimate is OK)</t>
+  </si>
+  <si>
+    <t>Please complete the table below indicating your weight at the specified time points. Please do not include weights during pregnancy, if applicable. At 18 weight unit of measure(Estimate is OK)</t>
+  </si>
+  <si>
+    <t>Please complete the table below indicating your weight at the specified time points. Please do not include weights during pregnancy, if applicable. At 18 weight Numerical value (Estimate is OK)</t>
+  </si>
+  <si>
+    <t>At what age were you at your highest weight? Please specify if in months or years.</t>
+  </si>
+  <si>
+    <t>Have you or your partner ever sought medical advice regarding fertility?</t>
   </si>
 </sst>
 </file>
@@ -1266,8 +1197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDA38AB1-F752-BB4E-9CFB-C6D8167B319F}">
   <dimension ref="A1:B57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1287,15 +1218,15 @@
     </row>
     <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>131</v>
+        <v>104</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>130</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>132</v>
+        <v>105</v>
       </c>
       <c r="B3" s="4">
         <v>123456</v>
@@ -1314,7 +1245,7 @@
         <v>63</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>133</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="51" x14ac:dyDescent="0.2">
@@ -1322,12 +1253,12 @@
         <v>64</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>134</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>135</v>
+        <v>108</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>3</v>
@@ -1335,7 +1266,7 @@
     </row>
     <row r="8" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>136</v>
+        <v>109</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>15</v>
@@ -1357,20 +1288,20 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B11" s="4" t="s">
+    </row>
+    <row r="12" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="B12" s="4" t="s">
         <v>70</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -1381,9 +1312,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>72</v>
+        <v>110</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>17</v>
@@ -1391,15 +1322,15 @@
     </row>
     <row r="15" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B16" s="4">
         <v>10</v>
@@ -1407,7 +1338,7 @@
     </row>
     <row r="17" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B17" s="4">
         <v>2004</v>
@@ -1421,70 +1352,73 @@
         <v>38301</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B19" s="7" t="s">
+    </row>
+    <row r="22" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+    <row r="24" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B24" s="4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+    <row r="25" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B25" s="4" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="85" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>38</v>
@@ -1492,36 +1426,39 @@
     </row>
     <row r="28" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="187" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>94</v>
+        <v>117</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="153" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>17</v>
@@ -1529,15 +1466,15 @@
     </row>
     <row r="33" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>17</v>
@@ -1545,180 +1482,186 @@
     </row>
     <row r="35" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="85" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
       <c r="B36" s="4">
         <v>4.5</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="102" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="B38" s="4">
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="102" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="8" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="B39" s="4">
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="85" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="8" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="85" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="8" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="8" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="8" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="8" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="85" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="8" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="B45" s="4">
         <v>70</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="8" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="136" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A47" s="8" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="B47" s="4">
         <v>128</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="136" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A48" s="8" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="B48" s="4">
         <v>130</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="136" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" s="8" t="s">
-        <v>120</v>
+        <v>134</v>
       </c>
       <c r="B49" s="4">
         <v>129</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="119" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A50" s="8" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="119" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A51" s="8" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="119" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="8" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="153" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="102" x14ac:dyDescent="0.2">
       <c r="A53" s="8" t="s">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" ht="153" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="102" x14ac:dyDescent="0.2">
       <c r="A54" s="8" t="s">
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="8" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="8" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="356" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" ht="187" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>129</v>
+        <v>102</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>